<commit_message>
Cree el reporte de la semana número 2 del ciclo 1
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/logt1/forma-logt1-20106065.xlsx
+++ b/tspi/ciclo-1/logt1/forma-logt1-20106065.xlsx
@@ -105,6 +105,7 @@
   <fonts count="6">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -125,11 +126,13 @@
     </font>
     <font>
       <name val="Times New Roman"/>
+      <charset val="1"/>
       <family val="1"/>
       <sz val="11"/>
     </font>
     <font>
       <name val="Times New Roman"/>
+      <charset val="1"/>
       <family val="1"/>
       <b val="true"/>
       <sz val="11"/>
@@ -262,21 +265,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E15" activeCellId="0" pane="topLeft" sqref="E15"/>
+      <selection activeCell="E16" activeCellId="0" pane="topLeft" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="12.2352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="17.0313725490196"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="11.2078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="17.4117647058824"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.2352941176471"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="48.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="12.2352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="17.1137254901961"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="11.2705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="17.5019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="48.4039215686275"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="12.2901960784314"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="1">
@@ -565,6 +568,12 @@
       </c>
       <c r="H14" s="6" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="16">
+      <c r="E16" s="3" t="n">
+        <f aca="false">SUM(E6:E14)/60</f>
+        <v>6.33333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>